<commit_message>
added columns, need to add logic
</commit_message>
<xml_diff>
--- a/shared/book.xlsx
+++ b/shared/book.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pineapple\IdeaProjects\IncompleteNightmare\shared\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03E92321-5BB5-4593-A2B5-0014AF1039AD}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4767CAC3-F4DA-441E-9BC0-9328A5F494FF}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7695" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="99">
   <si>
     <t>PST NAME</t>
   </si>
@@ -311,6 +311,12 @@
   </si>
   <si>
     <t>2018-10-23T18:53:54</t>
+  </si>
+  <si>
+    <t>Applied Rarities</t>
+  </si>
+  <si>
+    <t>Death Roll</t>
   </si>
 </sst>
 </file>
@@ -1172,10 +1178,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P45"/>
+  <dimension ref="A1:R45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1191,7 +1197,7 @@
     <col min="14" max="14" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1237,8 +1243,14 @@
       <c r="P1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q1" t="s">
+        <v>97</v>
+      </c>
+      <c r="R1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1284,7 +1296,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1330,7 +1342,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1376,7 +1388,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -1426,7 +1438,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -1472,7 +1484,7 @@
         <v>7.06</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1515,7 +1527,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1561,7 +1573,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1607,7 +1619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -1653,7 +1665,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -1699,7 +1711,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -1745,7 +1757,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -1791,7 +1803,7 @@
         <v>7.8999999999999995</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -1837,7 +1849,7 @@
         <v>8.2900000000000009</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>9</v>
       </c>
@@ -1884,7 +1896,7 @@
         <v>56.766666666666673</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>9</v>
       </c>

</xml_diff>